<commit_message>
generate the excel with all the children data
</commit_message>
<xml_diff>
--- a/Testing/B.xlsx
+++ b/Testing/B.xlsx
@@ -14,27 +14,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>Children Names</t>
   </si>
   <si>
-    <t xml:space="preserve">Max Time on response </t>
-  </si>
-  <si>
-    <t>paco</t>
-  </si>
-  <si>
-    <t>pepe</t>
-  </si>
-  <si>
-    <t>bea</t>
+    <t>Compleat Time(s)</t>
+  </si>
+  <si>
+    <t>Punctuation</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>Fails</t>
+  </si>
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>Paco</t>
+  </si>
+  <si>
+    <t>Pepe</t>
+  </si>
+  <si>
+    <t>Bea</t>
   </si>
   <si>
     <t>Rubén</t>
   </si>
   <si>
     <t>María</t>
+  </si>
+  <si>
+    <t>galdiolo</t>
+  </si>
+  <si>
+    <t>flor</t>
+  </si>
+  <si>
+    <t>palmera</t>
+  </si>
+  <si>
+    <t>bloso</t>
+  </si>
+  <si>
+    <t>Paco:</t>
+  </si>
+  <si>
+    <t>Pepe:</t>
+  </si>
+  <si>
+    <t>Bea:</t>
+  </si>
+  <si>
+    <t>Rubén:</t>
+  </si>
+  <si>
+    <t>María:</t>
   </si>
 </sst>
 </file>
@@ -366,58 +405,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C6"/>
+  <dimension ref="B1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="2:12">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:3">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="D2">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:3">
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>122</v>
+      </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="10:12">
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="10:12">
+      <c r="K18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="10:12">
+      <c r="K19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="10:12">
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="10:12">
+      <c r="J22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="10:12">
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="10:12">
+      <c r="K24" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="10:12">
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
genetate excel on a function
</commit_message>
<xml_diff>
--- a/Testing/B.xlsx
+++ b/Testing/B.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>Children Names</t>
   </si>
@@ -118,6 +118,194 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time on finish the game</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Random data</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$M$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sequential order</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Random jiggly bit values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,13 +593,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:12">
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +628,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:12">
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -463,7 +657,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -486,7 +683,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -509,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="1:12">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -532,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="1:12">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -543,7 +743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="1:12">
       <c r="J7" t="s">
         <v>16</v>
       </c>
@@ -554,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="1:12">
       <c r="K8" t="s">
         <v>12</v>
       </c>
@@ -562,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="1:12">
       <c r="K9" t="s">
         <v>13</v>
       </c>
@@ -570,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="1:12">
       <c r="K10" t="s">
         <v>14</v>
       </c>
@@ -578,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="1:12">
       <c r="J12" t="s">
         <v>17</v>
       </c>
@@ -589,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="1:12">
       <c r="K13" t="s">
         <v>12</v>
       </c>
@@ -597,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="1:12">
       <c r="K14" t="s">
         <v>13</v>
       </c>
@@ -605,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="1:12">
       <c r="K15" t="s">
         <v>14</v>
       </c>
@@ -685,5 +885,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
compleat parse the json file on children consoleç
</commit_message>
<xml_diff>
--- a/Testing/B.xlsx
+++ b/Testing/B.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>Children Names</t>
   </si>
@@ -118,194 +118,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Time on finish the game</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Random data</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$A$1:$M$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="50010001"/>
-        <c:axId val="50010002"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50010001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Sequential order</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50010002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Random jiggly bit values</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,16 +405,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="B1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
+    <row r="1" spans="2:12">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -628,10 +437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -657,10 +463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -683,10 +486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
+    <row r="4" spans="2:12">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -709,7 +509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -732,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -743,7 +543,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="2:12">
       <c r="J7" t="s">
         <v>16</v>
       </c>
@@ -754,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="2:12">
       <c r="K8" t="s">
         <v>12</v>
       </c>
@@ -762,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="2:12">
       <c r="K9" t="s">
         <v>13</v>
       </c>
@@ -770,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="2:12">
       <c r="K10" t="s">
         <v>14</v>
       </c>
@@ -778,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="2:12">
       <c r="J12" t="s">
         <v>17</v>
       </c>
@@ -789,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="2:12">
       <c r="K13" t="s">
         <v>12</v>
       </c>
@@ -797,7 +597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="2:12">
       <c r="K14" t="s">
         <v>13</v>
       </c>
@@ -805,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="2:12">
       <c r="K15" t="s">
         <v>14</v>
       </c>
@@ -885,6 +685,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
plot graph and enter image as background
</commit_message>
<xml_diff>
--- a/Testing/B.xlsx
+++ b/Testing/B.xlsx
@@ -118,6 +118,207 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Puntuación y tiempos de niños</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFC2"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -685,5 +886,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>